<commit_message>
update summary and notes
</commit_message>
<xml_diff>
--- a/ExploratorySessionNotes/ProjectSessionFiles/ProjectSession.xlsx
+++ b/ExploratorySessionNotes/ProjectSessionFiles/ProjectSession.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b24138e476aa9dbe/Documents/Studies/McGill/ECSE 429/Project/Part A/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="401" documentId="13_ncr:1_{76438F66-20F9-4164-B36D-2C14EAB23268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF97AB96-80F6-44E9-9AA9-C7968FD88FD4}"/>
+  <xr:revisionPtr revIDLastSave="636" documentId="13_ncr:1_{76438F66-20F9-4164-B36D-2C14EAB23268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{600F2BD1-C19A-42E9-BF75-C71605076182}"/>
   <bookViews>
-    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSessionNotes" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="174">
   <si>
     <t>Method</t>
   </si>
@@ -80,7 +80,7 @@
     <t>DOCUMENTED</t>
   </si>
   <si>
-    <t>return all instances of projects</t>
+    <t>return all instances of projects as json</t>
   </si>
   <si>
     <t>YES</t>
@@ -89,9 +89,21 @@
     <t>Same as expected</t>
   </si>
   <si>
+    <t>Accept: application/json</t>
+  </si>
+  <si>
     <t>1.png</t>
   </si>
   <si>
+    <t>return all instances of projects as xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same as expected </t>
+  </si>
+  <si>
+    <t>Accept: application/xml</t>
+  </si>
+  <si>
     <t>HEAD</t>
   </si>
   <si>
@@ -107,60 +119,129 @@
     <t>POST</t>
   </si>
   <si>
+    <t>UNDOCUMENTED</t>
+  </si>
+  <si>
     <t>we should be able to create project without a ID using the field values in the body of the message</t>
   </si>
   <si>
-    <t>400 bad request: not allowed to create with id,  successfully post after remove field id, Also cannot add multiple projects at once, only one project can be added at a time</t>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>400: "Failed Validation: completed should be BOOLEAN"</t>
+  </si>
+  <si>
+    <t>completed was a string</t>
   </si>
   <si>
     <t>3.png</t>
   </si>
   <si>
-    <t>/projects/id</t>
-  </si>
-  <si>
-    <t>return a specific instances of project using a id</t>
+    <t>400: "Not allowed to create with id"</t>
+  </si>
+  <si>
+    <t>id was not allowed</t>
+  </si>
+  <si>
+    <t>we should be able to create project without a ID using the field values in the body of the message, input and return the item in json</t>
+  </si>
+  <si>
+    <t>cannot add multiple projects at once, only one project can be added at a time</t>
+  </si>
+  <si>
+    <t>we should be able to create project without a ID using the field values in the body of the message, and return the item in xml</t>
+  </si>
+  <si>
+    <t>/projects/5</t>
+  </si>
+  <si>
+    <t>return a specific instances of project using a id as json</t>
   </si>
   <si>
     <t>4.png</t>
   </si>
   <si>
+    <t>return a specific instances of project using a id as xml</t>
+  </si>
+  <si>
+    <t>/projects/999</t>
+  </si>
+  <si>
+    <t>return a specific instances of project using an non existed id as json</t>
+  </si>
+  <si>
+    <t>"Could not find an instance with projects/999"</t>
+  </si>
+  <si>
     <t>amend a specific instances of project using a id with a body containing the fields to amend</t>
   </si>
   <si>
-    <t>400 bad request: not allowed to create with id,  successfully post after remove field id</t>
+    <t>400 bad request: not allowed to create with id</t>
+  </si>
+  <si>
+    <t>5.png</t>
+  </si>
+  <si>
+    <t>400 bad request: completed should be BOOLEAN</t>
+  </si>
+  <si>
+    <t>amend a specific instances of project using a id with a body containing the fields to amend, input and return in json</t>
   </si>
   <si>
     <t>It does not prevent user from adding project with existing id, when adding project with an existing id, it will replace the old project</t>
   </si>
   <si>
-    <t>5.png</t>
+    <t>amend a specific instances of project using a id with a body containing the fields to amend, input and return in xml</t>
+  </si>
+  <si>
+    <t>BUG</t>
   </si>
   <si>
     <t>PUT</t>
   </si>
   <si>
+    <t>amend a specific instances of project using a id with a body containing the fields to amend, input the body as json, return the result in json</t>
+  </si>
+  <si>
     <t>as expected</t>
   </si>
   <si>
     <t>6.png</t>
   </si>
   <si>
+    <t>amend a specific instances of project using a id with a body containing the fields to amend, input body as xml return the result in xml</t>
+  </si>
+  <si>
     <t>return headers for a specific instances of project using a id</t>
   </si>
   <si>
     <t>7.png</t>
   </si>
   <si>
-    <t>/projects/id/tasks</t>
-  </si>
-  <si>
-    <t>return all the todo items related to project, with given id, by the relationship named tasks</t>
+    <t>/projects/5/tasks</t>
+  </si>
+  <si>
+    <t>return all the todo items related to project, with given id, by the relationship named tasks, returned in json</t>
   </si>
   <si>
     <t>8.png</t>
   </si>
   <si>
+    <t>return all the todo items related to project, with given id, by the relationship named tasks, returned in xml</t>
+  </si>
+  <si>
+    <t>/projects/999/tasks</t>
+  </si>
+  <si>
+    <t>return all the todo items related to project, with non-existed id, by the relationship named tasks, returned in json</t>
+  </si>
+  <si>
+    <t>Everything to do item will be returned</t>
+  </si>
+  <si>
+    <t>16.png</t>
+  </si>
+  <si>
     <t>headers for the todo items related to project, with given id, by the relationship named tasks</t>
   </si>
   <si>
@@ -170,19 +251,25 @@
     <t>create an instance of a relationship named tasks between project instance :id and the todo instance represented by the id in the body of the message</t>
   </si>
   <si>
-    <t>400 bad request: not allowed to create with id, works as expected after remove id</t>
-  </si>
-  <si>
     <t>10.png</t>
   </si>
   <si>
-    <t>/projects/id/tasks/id</t>
+    <t>create an instance of a relationship named tasks between project instance :id and the todo instance represented by the id in the body of the message, input and return as xml</t>
+  </si>
+  <si>
+    <t>java.lang.IllegalStateException: Expected BEGIN_OBJECT but was STRING at line 1 column 1 path $</t>
+  </si>
+  <si>
+    <t>create an instance of a relationship named tasks between project instance :id and the todo instance represented by the id in the body of the message, input and return as json</t>
+  </si>
+  <si>
+    <t>/projects/3/tasks/5</t>
   </si>
   <si>
     <t>DELETE</t>
   </si>
   <si>
-    <t>delete the instance of the relationship named tasks between project and todo using the :id</t>
+    <t>delete the instance of the relationship named tasks between project and todo using an existing id</t>
   </si>
   <si>
     <t>Same as expected, use "GET" command to varify that the task is deleted</t>
@@ -194,15 +281,36 @@
     <t>11.png</t>
   </si>
   <si>
-    <t>/projects/id/categories</t>
-  </si>
-  <si>
-    <t>return all the category items related to project, with given id, by the relationship named categories</t>
+    <t>delete the instance of the relationship named tasks between project and todo using a non-existed id</t>
+  </si>
+  <si>
+    <t>"Could not find any instances with projects/8/tasks/2"</t>
+  </si>
+  <si>
+    <t>/projects/5/categories</t>
+  </si>
+  <si>
+    <t>return all the category items related to project, with given id, by the relationship named categories, input and return in json</t>
   </si>
   <si>
     <t>12.png</t>
   </si>
   <si>
+    <t>return all the category items related to project, with given id, by the relationship named categories, input and return in xml</t>
+  </si>
+  <si>
+    <t>/projects/999/categories</t>
+  </si>
+  <si>
+    <t>return all the category items related to project, with given non-existed id, by the relationship named categories, input and return in xml</t>
+  </si>
+  <si>
+    <t>All categries will be returned</t>
+  </si>
+  <si>
+    <t>17. png</t>
+  </si>
+  <si>
     <t>headers for the category items related to project, with given id, by the relationship named categories</t>
   </si>
   <si>
@@ -212,16 +320,19 @@
     <t>13.png</t>
   </si>
   <si>
-    <t>create an instance of a relationship named categories between project instance :id and the category instance represented by the id in the body of the message</t>
+    <t>create an instance of a relationship named categories between project instance :id and the category instance represented by the id in the body of the message, input and return as json</t>
   </si>
   <si>
     <t>14.png</t>
   </si>
   <si>
-    <t>/projects/id/categories/id</t>
-  </si>
-  <si>
-    <t>delete the instance of the relationship named categories between project and category using the :id</t>
+    <t>create an instance of a relationship named categories between project instance :id and the category instance represented by the id in the body of the message, input and return as xml</t>
+  </si>
+  <si>
+    <t>/projects/8/categories/5</t>
+  </si>
+  <si>
+    <t>delete the instance of the relationship named categories between project and category using an existing id</t>
   </si>
   <si>
     <t>Same as expected, use "GET" command to varify that the category is deleted</t>
@@ -233,7 +344,10 @@
     <t>15.png</t>
   </si>
   <si>
-    <t>BUG</t>
+    <t>delete the instance of the relationship named categories between project and category using the a non-existed id</t>
+  </si>
+  <si>
+    <t>"Could not find any instances with projects/5/categories/16"</t>
   </si>
   <si>
     <t>Expected Behavior</t>
@@ -258,16 +372,10 @@
     <t>Return all instances of todo, including new item</t>
   </si>
   <si>
-    <t>UNDOCUMENTED</t>
-  </si>
-  <si>
     <t>undocumented since ID is included in request body</t>
   </si>
   <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>400 bad request: not allowed to create with id</t>
   </si>
   <si>
     <t>added json body in request, including an ID</t>
@@ -585,7 +693,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -649,20 +757,19 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent2" xfId="1" builtinId="33"/>
@@ -1353,10 +1460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F59795-9E15-41F8-A389-D5EAAA170D5E}">
-  <dimension ref="A1:I998"/>
+  <dimension ref="A1:I997"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1"/>
@@ -1364,7 +1471,7 @@
     <col min="1" max="1" width="31" customWidth="1"/>
     <col min="2" max="2" width="12.125" customWidth="1"/>
     <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="37.125" style="28" customWidth="1"/>
+    <col min="4" max="4" width="37.125" customWidth="1"/>
     <col min="5" max="5" width="19.375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40.75" customWidth="1"/>
     <col min="7" max="7" width="31.75" customWidth="1"/>
@@ -1420,9 +1527,11 @@
       <c r="F2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="14" t="s">
+        <v>14</v>
+      </c>
       <c r="H2" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="16.5">
@@ -1430,7 +1539,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>10</v>
@@ -1444,12 +1553,12 @@
       <c r="F3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="11" t="s">
+      <c r="G3" s="14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="81">
+      <c r="H3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" ht="16.5">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -1466,114 +1575,112 @@
         <v>12</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="14" t="s">
         <v>21</v>
       </c>
+      <c r="G4" s="14"/>
       <c r="H4" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="32.25">
+    <row r="5" spans="1:9" ht="48.75">
       <c r="A5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="C5" s="7" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D5" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="48.75">
+      <c r="A6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="12" t="s">
+      <c r="D6" s="26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="64.5">
-      <c r="A6" s="7" t="s">
+      <c r="E6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" spans="1:9" ht="48.75">
+      <c r="A7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="30.75">
-      <c r="A7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>30</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="27" t="s">
-        <v>26</v>
+      <c r="D7" s="26" t="s">
+        <v>32</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="30.75">
+        <v>13</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="11"/>
+    </row>
+    <row r="8" spans="1:9" ht="48.75">
       <c r="A8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>15</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="24" t="s">
-        <v>33</v>
+      <c r="D8" s="26" t="s">
+        <v>34</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="30.75">
+        <v>13</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" spans="1:9" ht="32.25">
       <c r="A9" s="7" t="s">
         <v>35</v>
       </c>
@@ -1583,27 +1690,27 @@
       <c r="C9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="26" t="s">
         <v>36</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G9" s="14"/>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="12" t="s">
         <v>37</v>
       </c>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:9" ht="48.75">
+    <row r="10" spans="1:9" ht="32.25">
       <c r="A10" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>10</v>
@@ -1615,20 +1722,18 @@
         <v>12</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G10" s="14"/>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="12"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" ht="32.25">
+      <c r="A11" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" ht="64.5">
-      <c r="A11" s="7" t="s">
-        <v>35</v>
-      </c>
       <c r="B11" s="7" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>10</v>
@@ -1643,102 +1748,98 @@
         <v>41</v>
       </c>
       <c r="G11" s="14"/>
-      <c r="H11" s="12" t="s">
-        <v>42</v>
-      </c>
+      <c r="H11" s="12"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" ht="48.75">
       <c r="A12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="G12" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="12" t="s">
         <v>44</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>48</v>
       </c>
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9" ht="48.75">
       <c r="A13" s="7" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="12" t="s">
-        <v>51</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="12"/>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:9" ht="48.75">
+    <row r="14" spans="1:9" ht="64.5">
       <c r="A14" s="7" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>54</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="H14" s="12"/>
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" ht="64.5">
       <c r="A15" s="7" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>12</v>
@@ -1746,137 +1847,561 @@
       <c r="F15" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="I15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" ht="48.75">
+      <c r="G15" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="12"/>
+      <c r="I15" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="48.75" customHeight="1">
       <c r="A16" s="7" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="26" t="s">
-        <v>58</v>
+      <c r="D16" s="29" t="s">
+        <v>51</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F16" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="1:9" ht="61.5" customHeight="1">
+      <c r="A17" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="12"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="1:9" ht="45" customHeight="1">
+      <c r="A18" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="14"/>
+      <c r="H18" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9" ht="58.5" customHeight="1">
+      <c r="A19" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9" ht="69" customHeight="1">
+      <c r="A20" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="E20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="11"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" ht="61.5" customHeight="1">
+      <c r="A21" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="B21" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="24" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="17" spans="9:9" ht="15.75" customHeight="1">
-      <c r="I17" s="5"/>
-    </row>
-    <row r="18" spans="9:9" ht="15.75" customHeight="1">
-      <c r="I18" s="5"/>
-    </row>
-    <row r="19" spans="9:9" ht="15.75" customHeight="1">
-      <c r="I19" s="5"/>
-    </row>
-    <row r="20" spans="9:9" ht="15.75" customHeight="1">
-      <c r="I20" s="5"/>
-    </row>
-    <row r="21" spans="9:9" ht="15.75" customHeight="1">
+      <c r="E21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="14"/>
+      <c r="H21" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="I21" s="5"/>
     </row>
-    <row r="22" spans="9:9" ht="15.75" customHeight="1">
+    <row r="22" spans="1:9" ht="78" customHeight="1">
+      <c r="A22" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="14"/>
+      <c r="H22" s="11" t="s">
+        <v>66</v>
+      </c>
       <c r="I22" s="5"/>
     </row>
-    <row r="23" spans="9:9" ht="15.75" customHeight="1">
+    <row r="23" spans="1:9" ht="78" customHeight="1">
+      <c r="A23" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>68</v>
+      </c>
       <c r="I23" s="5"/>
     </row>
-    <row r="24" spans="9:9" ht="15.75" customHeight="1">
+    <row r="24" spans="1:9" ht="57" customHeight="1">
+      <c r="A24" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" s="14"/>
+      <c r="H24" s="12"/>
       <c r="I24" s="5"/>
     </row>
-    <row r="25" spans="9:9" ht="15.75" customHeight="1">
+    <row r="25" spans="1:9" ht="61.5" customHeight="1">
+      <c r="A25" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="12"/>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="9:9" ht="15.75" customHeight="1">
+    <row r="26" spans="1:9" ht="60.75" customHeight="1">
+      <c r="A26" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>77</v>
+      </c>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="9:9" ht="15.75" customHeight="1">
+    <row r="27" spans="1:9" ht="47.25" customHeight="1">
+      <c r="A27" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G27" s="14"/>
+      <c r="H27" s="12"/>
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="9:9" ht="15.75" customHeight="1">
+    <row r="28" spans="1:9" ht="81" customHeight="1">
+      <c r="A28" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>82</v>
+      </c>
       <c r="I28" s="5"/>
     </row>
-    <row r="29" spans="9:9" ht="15.75" customHeight="1">
+    <row r="29" spans="1:9" ht="83.25" customHeight="1">
+      <c r="A29" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H29" s="12"/>
       <c r="I29" s="5"/>
     </row>
-    <row r="30" spans="9:9" ht="15.75" customHeight="1">
+    <row r="30" spans="1:9" ht="79.5" customHeight="1">
+      <c r="A30" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="G30" s="14"/>
+      <c r="H30" s="12" t="s">
+        <v>87</v>
+      </c>
       <c r="I30" s="5"/>
     </row>
-    <row r="31" spans="9:9" ht="15.75" customHeight="1">
+    <row r="31" spans="1:9" ht="51.75" customHeight="1">
+      <c r="A31" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="9:9" ht="15.75" customHeight="1">
+    <row r="32" spans="1:9" ht="78" customHeight="1">
+      <c r="A32" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>92</v>
+      </c>
       <c r="I32" s="5"/>
     </row>
-    <row r="33" spans="9:9" ht="15.75" customHeight="1">
+    <row r="33" spans="1:9" ht="82.5" customHeight="1">
+      <c r="A33" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H33" s="11"/>
       <c r="I33" s="5"/>
     </row>
-    <row r="34" spans="9:9" ht="15.75" customHeight="1">
+    <row r="34" spans="1:9" ht="77.25" customHeight="1">
+      <c r="A34" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G34" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>98</v>
+      </c>
       <c r="I34" s="5"/>
     </row>
-    <row r="35" spans="9:9" ht="15.75" customHeight="1">
+    <row r="35" spans="1:9" ht="75.75" customHeight="1">
+      <c r="A35" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="G35" s="14"/>
+      <c r="H35" s="11"/>
       <c r="I35" s="5"/>
     </row>
-    <row r="36" spans="9:9" ht="15.75" customHeight="1">
+    <row r="36" spans="1:9" ht="15.75" customHeight="1">
       <c r="I36" s="5"/>
     </row>
-    <row r="37" spans="9:9" ht="15.75" customHeight="1">
+    <row r="37" spans="1:9" ht="15.75" customHeight="1">
       <c r="I37" s="5"/>
     </row>
-    <row r="38" spans="9:9" ht="15.75" customHeight="1">
+    <row r="38" spans="1:9" ht="15.75" customHeight="1">
       <c r="I38" s="5"/>
     </row>
-    <row r="39" spans="9:9" ht="15.75" customHeight="1">
+    <row r="39" spans="1:9" ht="15.75" customHeight="1">
       <c r="I39" s="5"/>
     </row>
-    <row r="40" spans="9:9" ht="15.75" customHeight="1">
+    <row r="40" spans="1:9" ht="15.75" customHeight="1">
       <c r="I40" s="5"/>
     </row>
-    <row r="41" spans="9:9" ht="15.75" customHeight="1">
+    <row r="41" spans="1:9" ht="15.75" customHeight="1">
       <c r="I41" s="5"/>
     </row>
-    <row r="42" spans="9:9" ht="15.75" customHeight="1">
+    <row r="42" spans="1:9" ht="15.75" customHeight="1">
       <c r="I42" s="5"/>
     </row>
-    <row r="43" spans="9:9" ht="15.75" customHeight="1">
+    <row r="43" spans="1:9" ht="15.75" customHeight="1">
       <c r="I43" s="5"/>
     </row>
-    <row r="44" spans="9:9" ht="15.75" customHeight="1">
+    <row r="44" spans="1:9" ht="15.75" customHeight="1">
       <c r="I44" s="5"/>
     </row>
-    <row r="45" spans="9:9" ht="15.75" customHeight="1">
+    <row r="45" spans="1:9" ht="15.75" customHeight="1">
       <c r="I45" s="5"/>
     </row>
-    <row r="46" spans="9:9" ht="15.75" customHeight="1">
+    <row r="46" spans="1:9" ht="15.75" customHeight="1">
       <c r="I46" s="5"/>
     </row>
-    <row r="47" spans="9:9" ht="15.75" customHeight="1">
+    <row r="47" spans="1:9" ht="15.75" customHeight="1">
       <c r="I47" s="5"/>
     </row>
-    <row r="48" spans="9:9" ht="15.75" customHeight="1">
-      <c r="I48" s="5"/>
-    </row>
+    <row r="48" spans="1:9" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -2826,10 +3351,9 @@
     <row r="995" ht="15.75" customHeight="1"/>
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="B1:B98">
+  <conditionalFormatting sqref="B1:B117">
     <cfRule type="cellIs" dxfId="49" priority="1" operator="equal">
       <formula>"PATCH"</formula>
     </cfRule>
@@ -2852,7 +3376,7 @@
       <formula>"PUT"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C98">
+  <conditionalFormatting sqref="C1:C117">
     <cfRule type="cellIs" dxfId="42" priority="8" operator="equal">
       <formula>"DOCUMENTED"</formula>
     </cfRule>
@@ -2860,7 +3384,7 @@
       <formula>"UNDOCUMENTED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C99:C998">
+  <conditionalFormatting sqref="C118:C1017">
     <cfRule type="cellIs" dxfId="40" priority="13" operator="equal">
       <formula>"PATCH"</formula>
     </cfRule>
@@ -2883,12 +3407,12 @@
       <formula>"PUT"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D98">
+  <conditionalFormatting sqref="D2:D117">
     <cfRule type="cellIs" dxfId="33" priority="25" stopIfTrue="1" operator="equal">
       <formula>"method not allowed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D99:D998">
+  <conditionalFormatting sqref="D118:D1017">
     <cfRule type="cellIs" dxfId="32" priority="20" operator="equal">
       <formula>"DOCUMENTED"</formula>
     </cfRule>
@@ -2896,7 +3420,7 @@
       <formula>"UNDOCUMENTED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E98">
+  <conditionalFormatting sqref="E1:E117">
     <cfRule type="cellIs" dxfId="30" priority="10" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
@@ -2907,7 +3431,7 @@
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F99:F998">
+  <conditionalFormatting sqref="F118:F1017">
     <cfRule type="cellIs" dxfId="27" priority="22" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
@@ -2919,16 +3443,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" sqref="D2:D98" xr:uid="{166FEC60-EE6A-4FBF-B394-650198DA1992}">
+    <dataValidation type="list" allowBlank="1" sqref="D2:D117" xr:uid="{166FEC60-EE6A-4FBF-B394-650198DA1992}">
       <formula1>"method not allowed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C98" xr:uid="{91E71026-4060-4C08-AD7E-CE16BE367240}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C117" xr:uid="{91E71026-4060-4C08-AD7E-CE16BE367240}">
       <formula1>"UNDOCUMENTED,DOCUMENTED"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:B98" xr:uid="{EE1EA7D4-B04D-4CD5-9A55-439BB7D8BB75}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:B117" xr:uid="{EE1EA7D4-B04D-4CD5-9A55-439BB7D8BB75}">
       <formula1>"GET,PUT,POST,DELETE,OPTIONS,HEAD,PATCH"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E98" xr:uid="{3C87F2DB-0B4C-42AF-A4F6-E69734FD7D04}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E117" xr:uid="{3C87F2DB-0B4C-42AF-A4F6-E69734FD7D04}">
       <formula1>"YES,NO,N/A"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2972,7 +3496,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>63</v>
+        <v>101</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>4</v>
@@ -2989,7 +3513,7 @@
     </row>
     <row r="2" spans="1:9" ht="15.6">
       <c r="A2" s="7" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>9</v>
@@ -2998,7 +3522,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>65</v>
+        <v>103</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>12</v>
@@ -3008,45 +3532,45 @@
       </c>
       <c r="G2" s="14"/>
       <c r="H2" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.6">
       <c r="A3" s="7" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>66</v>
+        <v>104</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G3" s="14"/>
       <c r="H3" s="11" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.6">
       <c r="A4" s="7" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>12</v>
@@ -3055,15 +3579,15 @@
         <v>13</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="31.15">
       <c r="A5" s="7" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>9</v>
@@ -3072,7 +3596,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>12</v>
@@ -3085,92 +3609,92 @@
     </row>
     <row r="6" spans="1:9" ht="31.15">
       <c r="A6" s="7" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>71</v>
+        <v>108</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.6">
       <c r="A7" s="7" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>75</v>
+        <v>111</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="12"/>
     </row>
     <row r="8" spans="1:9" ht="15.6">
       <c r="A8" s="7" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>75</v>
+        <v>111</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="11"/>
     </row>
     <row r="9" spans="1:9" ht="15.6">
       <c r="A9" s="7" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>76</v>
+        <v>112</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>75</v>
+        <v>111</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="11"/>
@@ -3178,34 +3702,34 @@
     </row>
     <row r="10" spans="1:9" ht="31.15">
       <c r="A10" s="7" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>77</v>
+        <v>113</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" ht="15.6">
       <c r="A11" s="7" t="s">
-        <v>81</v>
+        <v>117</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>9</v>
@@ -3214,7 +3738,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>82</v>
+        <v>118</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>12</v>
@@ -3224,22 +3748,22 @@
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="12" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" ht="15.6">
       <c r="A12" s="7" t="s">
-        <v>81</v>
+        <v>117</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>83</v>
+        <v>119</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>12</v>
@@ -3249,22 +3773,22 @@
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="13" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9" ht="15.6">
       <c r="A13" s="7" t="s">
-        <v>81</v>
+        <v>117</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>84</v>
+        <v>120</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>12</v>
@@ -3273,52 +3797,52 @@
         <v>13</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>85</v>
+        <v>121</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:9" ht="31.15">
       <c r="A14" s="7" t="s">
-        <v>86</v>
+        <v>122</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>87</v>
+        <v>123</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>88</v>
+        <v>124</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:9" ht="15.6">
       <c r="A15" s="7" t="s">
-        <v>81</v>
+        <v>117</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>89</v>
+        <v>125</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>12</v>
@@ -3332,36 +3856,36 @@
     </row>
     <row r="16" spans="1:9" ht="62.45">
       <c r="A16" s="7" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>90</v>
+        <v>126</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>92</v>
+        <v>128</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="46.9">
       <c r="A17" s="7" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>9</v>
@@ -3370,7 +3894,7 @@
         <v>10</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>12</v>
@@ -3379,16 +3903,16 @@
         <v>13</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>94</v>
+        <v>130</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="I17" s="5"/>
     </row>
     <row r="18" spans="1:9" ht="31.15">
       <c r="A18" s="7" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>9</v>
@@ -3397,7 +3921,7 @@
         <v>10</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>12</v>
@@ -3406,10 +3930,10 @@
         <v>13</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="I18" s="5"/>
     </row>
@@ -6029,10 +6553,10 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
       <c r="A1" s="6" t="s">
-        <v>96</v>
+        <v>132</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>97</v>
+        <v>133</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -6043,7 +6567,7 @@
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>98</v>
+        <v>134</v>
       </c>
       <c r="B2" s="17">
         <v>261032441</v>
@@ -6057,10 +6581,10 @@
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1">
       <c r="A3" s="9" t="s">
-        <v>99</v>
+        <v>135</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>100</v>
+        <v>136</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -6071,7 +6595,7 @@
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>137</v>
       </c>
       <c r="B4" s="18">
         <v>45568</v>
@@ -6085,10 +6609,10 @@
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>138</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>103</v>
+        <v>139</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -6108,10 +6632,10 @@
     </row>
     <row r="7" spans="1:8" ht="16.5">
       <c r="A7" s="3" t="s">
-        <v>104</v>
+        <v>140</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>105</v>
+        <v>141</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -6123,7 +6647,7 @@
     <row r="8" spans="1:8" ht="32.25">
       <c r="A8" s="2"/>
       <c r="B8" s="20" t="s">
-        <v>106</v>
+        <v>142</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -6135,7 +6659,7 @@
     <row r="9" spans="1:8" ht="32.25">
       <c r="A9" s="2"/>
       <c r="B9" s="20" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -6147,7 +6671,7 @@
     <row r="10" spans="1:8" ht="31.15">
       <c r="A10" s="2"/>
       <c r="B10" s="20" t="s">
-        <v>108</v>
+        <v>144</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -6159,7 +6683,7 @@
     <row r="11" spans="1:8" ht="31.15">
       <c r="A11" s="2"/>
       <c r="B11" s="20" t="s">
-        <v>109</v>
+        <v>145</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -6180,10 +6704,10 @@
     </row>
     <row r="13" spans="1:8" ht="32.25">
       <c r="A13" s="21" t="s">
-        <v>110</v>
+        <v>146</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>111</v>
+        <v>147</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -6195,7 +6719,7 @@
     <row r="14" spans="1:8" ht="32.25">
       <c r="A14" s="2"/>
       <c r="B14" s="20" t="s">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -6207,7 +6731,7 @@
     <row r="15" spans="1:8" ht="16.5">
       <c r="A15" s="2"/>
       <c r="B15" s="20" t="s">
-        <v>113</v>
+        <v>149</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -6218,7 +6742,7 @@
     </row>
     <row r="16" spans="1:8" ht="31.15">
       <c r="B16" s="20" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -6230,7 +6754,7 @@
     <row r="17" spans="1:8" ht="15" customHeight="1">
       <c r="A17" s="2"/>
       <c r="B17" s="1" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -6241,10 +6765,10 @@
     </row>
     <row r="18" spans="1:8" ht="48.75">
       <c r="A18" s="21" t="s">
-        <v>116</v>
+        <v>152</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -6265,10 +6789,10 @@
     </row>
     <row r="20" spans="1:8" ht="16.5">
       <c r="A20" s="3" t="s">
-        <v>118</v>
+        <v>154</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -6280,7 +6804,7 @@
     <row r="21" spans="1:8" ht="16.5">
       <c r="A21" s="2"/>
       <c r="B21" s="19" t="s">
-        <v>120</v>
+        <v>156</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -6292,7 +6816,7 @@
     <row r="22" spans="1:8" ht="16.5">
       <c r="A22" s="2"/>
       <c r="B22" s="20" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -6303,7 +6827,7 @@
     </row>
     <row r="23" spans="1:8" ht="16.5">
       <c r="B23" s="20" t="s">
-        <v>122</v>
+        <v>158</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -6314,7 +6838,7 @@
     </row>
     <row r="24" spans="1:8" ht="32.25">
       <c r="B24" s="22" t="s">
-        <v>123</v>
+        <v>159</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -6326,7 +6850,7 @@
     <row r="25" spans="1:8" ht="15" customHeight="1">
       <c r="A25" s="2"/>
       <c r="B25" s="1" t="s">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -6340,8 +6864,8 @@
       <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1">
-      <c r="A27" s="29"/>
-      <c r="B27" s="30"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="28"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -6371,10 +6895,10 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
       <c r="A1" s="6" t="s">
-        <v>96</v>
+        <v>132</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>125</v>
+        <v>161</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -6385,7 +6909,7 @@
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>98</v>
+        <v>134</v>
       </c>
       <c r="B2" s="17">
         <v>261059531</v>
@@ -6399,10 +6923,10 @@
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1">
       <c r="A3" s="9" t="s">
-        <v>99</v>
+        <v>135</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -6413,7 +6937,7 @@
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>137</v>
       </c>
       <c r="B4" s="18">
         <v>45567</v>
@@ -6427,10 +6951,10 @@
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>138</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>127</v>
+        <v>163</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -6450,10 +6974,10 @@
     </row>
     <row r="7" spans="1:8" ht="15.6">
       <c r="A7" s="3" t="s">
-        <v>104</v>
+        <v>140</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>128</v>
+        <v>164</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -6465,7 +6989,7 @@
     <row r="8" spans="1:8" ht="31.15">
       <c r="A8" s="2"/>
       <c r="B8" s="20" t="s">
-        <v>129</v>
+        <v>165</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -6477,7 +7001,7 @@
     <row r="9" spans="1:8" ht="31.15">
       <c r="A9" s="2"/>
       <c r="B9" s="20" t="s">
-        <v>130</v>
+        <v>166</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -6489,7 +7013,7 @@
     <row r="10" spans="1:8" ht="31.15">
       <c r="A10" s="2"/>
       <c r="B10" s="20" t="s">
-        <v>108</v>
+        <v>144</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -6501,7 +7025,7 @@
     <row r="11" spans="1:8" ht="31.15">
       <c r="A11" s="2"/>
       <c r="B11" s="20" t="s">
-        <v>109</v>
+        <v>145</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -6522,10 +7046,10 @@
     </row>
     <row r="13" spans="1:8" ht="31.15">
       <c r="A13" s="21" t="s">
-        <v>110</v>
+        <v>146</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>131</v>
+        <v>167</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -6537,7 +7061,7 @@
     <row r="14" spans="1:8" ht="31.15">
       <c r="A14" s="2"/>
       <c r="B14" s="20" t="s">
-        <v>132</v>
+        <v>168</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -6549,7 +7073,7 @@
     <row r="15" spans="1:8" ht="15.6">
       <c r="A15" s="2"/>
       <c r="B15" s="20" t="s">
-        <v>133</v>
+        <v>169</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -6560,7 +7084,7 @@
     </row>
     <row r="16" spans="1:8" ht="31.15">
       <c r="B16" s="20" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -6581,10 +7105,10 @@
     </row>
     <row r="18" spans="1:8" ht="46.9">
       <c r="A18" s="21" t="s">
-        <v>116</v>
+        <v>152</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -6605,10 +7129,10 @@
     </row>
     <row r="20" spans="1:8" ht="15.6">
       <c r="A20" s="3" t="s">
-        <v>118</v>
+        <v>154</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -6620,7 +7144,7 @@
     <row r="21" spans="1:8" ht="15.6">
       <c r="A21" s="2"/>
       <c r="B21" s="19" t="s">
-        <v>134</v>
+        <v>170</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -6632,7 +7156,7 @@
     <row r="22" spans="1:8" ht="15.6">
       <c r="A22" s="2"/>
       <c r="B22" s="20" t="s">
-        <v>135</v>
+        <v>171</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -6643,7 +7167,7 @@
     </row>
     <row r="23" spans="1:8" ht="15.6">
       <c r="B23" s="20" t="s">
-        <v>136</v>
+        <v>172</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -6654,7 +7178,7 @@
     </row>
     <row r="24" spans="1:8" ht="31.15">
       <c r="B24" s="22" t="s">
-        <v>137</v>
+        <v>173</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -6677,8 +7201,8 @@
       <c r="B26" s="1"/>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1">
-      <c r="A27" s="29"/>
-      <c r="B27" s="30"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="28"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>